<commit_message>
injection results - added average air pressure
</commit_message>
<xml_diff>
--- a/Injections/Injections_Results/Inj_results_2022-06-06.xlsx
+++ b/Injections/Injections_Results/Inj_results_2022-06-06.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kriddie/Documents/Ecuador2022/Injections/Injections_Results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1ABE69D-000B-9646-9290-DF678D0420E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{885B990C-85E8-BD49-8435-AF3023D48AA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8200" yWindow="3000" windowWidth="27640" windowHeight="16940" xr2:uid="{B537B67D-4336-9741-9AE0-B632B4F45081}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Date</t>
   </si>
@@ -171,6 +171,9 @@
   </si>
   <si>
     <t>slope btw 0 and 50</t>
+  </si>
+  <si>
+    <t>Ave Air Press (kPa)</t>
   </si>
 </sst>
 </file>
@@ -563,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{173AACA0-6003-0B4F-96CA-34FCF7DDAFB1}">
-  <dimension ref="A1:I37"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -880,47 +883,57 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="B33" s="3">
-        <v>1.3520000000000001</v>
+        <v>45</v>
+      </c>
+      <c r="B33">
+        <v>64.430000000000007</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B34" s="3">
-        <v>8.2050000000000001</v>
+        <v>1.3520000000000001</v>
       </c>
       <c r="D34" s="7"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B35" s="3">
-        <v>10.199</v>
+        <v>8.2050000000000001</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="5"/>
+        <v>38</v>
+      </c>
+      <c r="B36" s="3">
+        <v>10.199</v>
+      </c>
       <c r="D36" s="7"/>
+      <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B37" s="5"/>
       <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B38" s="5"/>
+      <c r="D38" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>